<commit_message>
updated board and BOM with rev1.1 notes
</commit_message>
<xml_diff>
--- a/oresat-camera-hardware/star-tracker-card/star-tracker-card-eagle-bom.xlsx
+++ b/oresat-camera-hardware/star-tracker-card/star-tracker-card-eagle-bom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oliver.rew/github/oresat-star-tracker/oresat-camera-hardware/star-tracker-card/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oliver.rew/oresat/oresat-star-tracker/oresat-camera-hardware/star-tracker-card/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ECF255E-3C8D-C147-8F0C-3EDB2A3B4A66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1158730-9ACC-E242-B015-9EF717E71ACB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2140" yWindow="2560" windowWidth="30940" windowHeight="16440" xr2:uid="{D8C2B724-F8B5-8341-8BE4-D938CAE2AF6E}"/>
+    <workbookView xWindow="10860" yWindow="460" windowWidth="30940" windowHeight="16440" xr2:uid="{D8C2B724-F8B5-8341-8BE4-D938CAE2AF6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -666,7 +666,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1027,19 +1027,19 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F30" sqref="F30"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
     <col min="3" max="3" width="33" customWidth="1"/>
     <col min="4" max="4" width="30.83203125" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" customWidth="1"/>
+    <col min="5" max="5" width="94.5" customWidth="1"/>
     <col min="6" max="6" width="25.83203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="3" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1114,7 +1114,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1137,7 +1137,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1160,7 +1160,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1183,7 +1183,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1206,7 +1206,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1229,7 +1229,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1255,7 +1255,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1278,7 +1278,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1301,7 +1301,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1324,7 +1324,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1350,7 +1350,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1376,7 +1376,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1399,7 +1399,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1422,7 +1422,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1445,7 +1445,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1471,7 +1471,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1497,7 +1497,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8">
       <c r="A20">
         <v>2</v>
       </c>
@@ -1523,7 +1523,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1546,7 +1546,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1569,7 +1569,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8">
       <c r="A23">
         <v>1</v>
       </c>
@@ -1595,7 +1595,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1618,7 +1618,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8">
       <c r="A25">
         <v>1</v>
       </c>
@@ -1641,7 +1641,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1664,7 +1664,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8">
       <c r="A27">
         <v>3</v>
       </c>
@@ -1687,7 +1687,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8">
       <c r="A28">
         <v>3</v>
       </c>
@@ -1710,7 +1710,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1733,7 +1733,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1756,7 +1756,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8">
       <c r="A31">
         <v>5</v>
       </c>
@@ -1776,7 +1776,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8">
       <c r="A32">
         <v>4</v>
       </c>
@@ -1796,7 +1796,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6">
       <c r="A33">
         <v>4</v>
       </c>
@@ -1816,7 +1816,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6">
       <c r="A34">
         <v>10</v>
       </c>
@@ -1836,7 +1836,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6">
       <c r="A35">
         <v>2</v>
       </c>
@@ -1856,7 +1856,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6">
       <c r="A36">
         <v>14</v>
       </c>
@@ -1876,7 +1876,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6">
       <c r="A37">
         <v>3</v>
       </c>
@@ -1896,7 +1896,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6">
       <c r="A38">
         <v>4</v>
       </c>
@@ -1916,7 +1916,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6">
       <c r="A39">
         <v>1</v>
       </c>
@@ -1936,7 +1936,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6">
       <c r="A40">
         <v>5</v>
       </c>
@@ -1956,7 +1956,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6">
       <c r="A41">
         <v>3</v>
       </c>
@@ -1976,7 +1976,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6">
       <c r="A42">
         <v>4</v>
       </c>
@@ -1996,7 +1996,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6">
       <c r="A43">
         <v>1</v>
       </c>
@@ -2016,7 +2016,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6">
       <c r="A44">
         <v>1</v>
       </c>
@@ -2036,7 +2036,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6">
       <c r="A45">
         <v>2</v>
       </c>
@@ -2056,7 +2056,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6">
       <c r="A46">
         <v>3</v>
       </c>
@@ -2076,7 +2076,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6">
       <c r="A47">
         <v>2</v>
       </c>
@@ -2096,7 +2096,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6">
       <c r="A48">
         <v>3</v>
       </c>
@@ -2116,7 +2116,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6">
       <c r="A49">
         <v>21</v>
       </c>
@@ -2136,7 +2136,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6">
       <c r="A50">
         <v>1</v>
       </c>

</xml_diff>